<commit_message>
Atualização da Documentação: -3º seminario -Casos de teste
</commit_message>
<xml_diff>
--- a/Documentação/Casos de Teste (1-20).xlsx
+++ b/Documentação/Casos de Teste (1-20).xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visagio\git\BatalhaDoPassinho\Documentação\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
@@ -31,9 +36,6 @@
     <t xml:space="preserve"> Adição de tropas iniciais</t>
   </si>
   <si>
-    <t xml:space="preserve"> Remanejamento de tropas para país vizinho aliado</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Remanejamento de tropas para país vizinho inimigo</t>
   </si>
   <si>
@@ -309,13 +311,16 @@
   </si>
   <si>
     <t>IA distribui um território</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Remanejamento de tropas para território vizinho aliado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,16 +645,16 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -658,16 +663,16 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -699,6 +704,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -747,7 +755,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,9 +787,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -813,6 +822,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -988,14 +998,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -1004,1361 +1014,1425 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="12">
+        <v>14</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="2:4">
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="2:4">
+      <c r="C3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="2:4">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" s="3" customFormat="1">
+    </row>
+    <row r="6" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="9" spans="2:4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="12">
+        <v>14</v>
+      </c>
+      <c r="C9" s="14">
         <v>2</v>
       </c>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="2:4">
+      <c r="C10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="2:4">
+        <v>13</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" s="3" customFormat="1">
+    </row>
+    <row r="13" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" s="3" customFormat="1" ht="25.5">
+    </row>
+    <row r="14" spans="2:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
         <v>2</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="12">
+        <v>14</v>
+      </c>
+      <c r="C17" s="14">
         <v>3</v>
       </c>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="C18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:5">
+        <v>13</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="3" customFormat="1">
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
         <v>1</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" ht="38.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>2</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="25" spans="1:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="12">
+        <v>14</v>
+      </c>
+      <c r="C25" s="14">
         <v>4</v>
       </c>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="C26" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1">
+        <v>13</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1">
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
         <v>1</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="25.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
         <v>2</v>
       </c>
       <c r="C30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="12">
+        <v>14</v>
+      </c>
+      <c r="C33" s="14">
         <v>5</v>
       </c>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="2:4">
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="2:4">
+      <c r="C34" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="15"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
     </row>
-    <row r="36" spans="2:4" s="3" customFormat="1">
+    <row r="36" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="8">
         <v>1</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="25.5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8">
         <v>2</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="25.5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B39" s="8">
         <v>3</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="8">
         <v>4</v>
       </c>
       <c r="C40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4">
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="8">
         <v>5</v>
       </c>
       <c r="C41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="8">
         <v>6</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="25.5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B43" s="8">
         <v>7</v>
       </c>
       <c r="C43" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44" s="14"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="2:4">
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="12"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="12">
+        <v>14</v>
+      </c>
+      <c r="C46" s="14">
         <v>6</v>
       </c>
-      <c r="D46" s="13"/>
-    </row>
-    <row r="47" spans="2:4">
+      <c r="D46" s="15"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="15"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="13"/>
-    </row>
-    <row r="48" spans="2:4">
-      <c r="B48" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="C48" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D48" s="17"/>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" s="3" customFormat="1" ht="25.5">
+    </row>
+    <row r="50" spans="2:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B50" s="6">
         <v>1</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="14"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="53" spans="2:4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="12"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="12">
+        <v>14</v>
+      </c>
+      <c r="C53" s="14">
         <v>7</v>
       </c>
-      <c r="D53" s="13"/>
-    </row>
-    <row r="54" spans="2:4">
+      <c r="D53" s="15"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="13"/>
-    </row>
-    <row r="55" spans="2:4">
+      <c r="C54" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="15"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D55" s="17"/>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="D56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" s="3" customFormat="1" ht="38.25">
+    </row>
+    <row r="57" spans="2:4" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B57" s="6">
         <v>1</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" s="3" customFormat="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
     </row>
-    <row r="59" spans="2:4">
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-    </row>
-    <row r="60" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="12">
+        <v>14</v>
+      </c>
+      <c r="C60" s="14">
         <v>8</v>
       </c>
-      <c r="D60" s="13"/>
-    </row>
-    <row r="61" spans="2:4">
+      <c r="D60" s="15"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="13"/>
-    </row>
-    <row r="62" spans="2:4" ht="30.75" customHeight="1">
+      <c r="D61" s="15"/>
+    </row>
+    <row r="62" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D62" s="17"/>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="D63" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" s="3" customFormat="1" ht="25.5">
+    </row>
+    <row r="64" spans="2:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B64" s="6">
         <v>1</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" s="3" customFormat="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="6">
         <v>2</v>
       </c>
       <c r="C65" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" s="3" customFormat="1" ht="25.5">
+    </row>
+    <row r="66" spans="2:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B66" s="6">
         <v>3</v>
       </c>
       <c r="C66" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D66" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4">
-      <c r="B67" s="14"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-    </row>
-    <row r="69" spans="2:4">
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="12"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="12">
+        <v>14</v>
+      </c>
+      <c r="C69" s="14">
         <v>9</v>
       </c>
-      <c r="D69" s="13"/>
-    </row>
-    <row r="70" spans="2:4">
+      <c r="D69" s="15"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="C70" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="13"/>
-    </row>
-    <row r="71" spans="2:4">
+      <c r="D70" s="15"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D71" s="17"/>
     </row>
-    <row r="72" spans="2:4">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="D72" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" s="3" customFormat="1" ht="25.5">
+    </row>
+    <row r="73" spans="2:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B73" s="6">
         <v>1</v>
       </c>
       <c r="C73" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4">
-      <c r="B74" s="14"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-    </row>
-    <row r="76" spans="2:4">
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="12"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" s="12">
+        <v>14</v>
+      </c>
+      <c r="C76" s="14">
         <v>10</v>
       </c>
-      <c r="D76" s="13"/>
-    </row>
-    <row r="77" spans="2:4">
+      <c r="D76" s="15"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C77" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="13"/>
-    </row>
-    <row r="78" spans="2:4" ht="27" customHeight="1">
+      <c r="D77" s="15"/>
+    </row>
+    <row r="78" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D78" s="17"/>
     </row>
-    <row r="79" spans="2:4">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="D79" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" s="3" customFormat="1">
+    </row>
+    <row r="80" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6">
         <v>1</v>
       </c>
       <c r="C80" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" s="3" customFormat="1" ht="25.5">
+    </row>
+    <row r="81" spans="2:4" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B81" s="6">
         <v>2</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4">
-      <c r="B82" s="14"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
-    </row>
-    <row r="84" spans="2:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="12"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" s="12">
+        <v>14</v>
+      </c>
+      <c r="C84" s="14">
         <v>11</v>
       </c>
-      <c r="D84" s="13"/>
-    </row>
-    <row r="85" spans="2:4">
+      <c r="D84" s="15"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C85" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="13"/>
-    </row>
-    <row r="86" spans="2:4">
+      <c r="D85" s="15"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D86" s="17"/>
     </row>
-    <row r="87" spans="2:4">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="D87" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D87" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" ht="38.25">
+    </row>
+    <row r="88" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B88" s="6">
         <v>1</v>
       </c>
       <c r="C88" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" s="3" customFormat="1">
+    </row>
+    <row r="89" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="6">
         <v>2</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4">
-      <c r="B90" s="14"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-    </row>
-    <row r="92" spans="2:4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="12"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C92" s="12">
+        <v>14</v>
+      </c>
+      <c r="C92" s="14">
         <v>12</v>
       </c>
-      <c r="D92" s="13"/>
-    </row>
-    <row r="93" spans="2:4">
+      <c r="D92" s="15"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C93" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D93" s="13"/>
-    </row>
-    <row r="94" spans="2:4" ht="42.75" customHeight="1">
+      <c r="C93" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D93" s="15"/>
+    </row>
+    <row r="94" spans="2:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D94" s="17"/>
     </row>
-    <row r="95" spans="2:4">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="D95" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4" s="3" customFormat="1" ht="38.25">
+    </row>
+    <row r="96" spans="2:4" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B96" s="6">
         <v>1</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4">
-      <c r="B97" s="14"/>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
-    </row>
-    <row r="99" spans="2:4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="12"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C99" s="12">
+        <v>14</v>
+      </c>
+      <c r="C99" s="14">
         <v>13</v>
       </c>
-      <c r="D99" s="13"/>
-    </row>
-    <row r="100" spans="2:4">
+      <c r="D99" s="15"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C100" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D100" s="13"/>
-    </row>
-    <row r="101" spans="2:4" s="3" customFormat="1" ht="30.75" customHeight="1">
+      <c r="C100" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D100" s="15"/>
+    </row>
+    <row r="101" spans="2:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C101" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D101" s="17"/>
     </row>
-    <row r="102" spans="2:4">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="D102" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D102" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" ht="25.5">
+    </row>
+    <row r="103" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B103" s="6">
         <v>1</v>
       </c>
       <c r="C103" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D103" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D103" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" ht="25.5">
+    </row>
+    <row r="104" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B104" s="6">
         <v>2</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" ht="25.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B105" s="6">
         <v>3</v>
       </c>
       <c r="C105" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D105" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" ht="25.5">
+    </row>
+    <row r="106" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B106" s="6">
         <v>4</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" s="3" customFormat="1">
-      <c r="B107" s="14"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-    </row>
-    <row r="109" spans="2:4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="12"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C109" s="12">
         <v>14</v>
       </c>
-      <c r="D109" s="13"/>
-    </row>
-    <row r="110" spans="2:4">
+      <c r="C109" s="14">
+        <v>14</v>
+      </c>
+      <c r="D109" s="15"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C110" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D110" s="13"/>
-    </row>
-    <row r="111" spans="2:4" s="3" customFormat="1" ht="30.75" customHeight="1">
+      <c r="C110" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" s="15"/>
+    </row>
+    <row r="111" spans="2:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D111" s="17"/>
     </row>
-    <row r="112" spans="2:4">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="D112" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D112" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" ht="25.5">
+    </row>
+    <row r="113" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B113" s="6">
         <v>1</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" s="3" customFormat="1">
-      <c r="B114" s="14"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="15"/>
-    </row>
-    <row r="115" spans="2:4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="12"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="2:4">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C116" s="14">
         <v>15</v>
       </c>
-      <c r="C116" s="12">
-        <v>15</v>
-      </c>
-      <c r="D116" s="13"/>
-    </row>
-    <row r="117" spans="2:4">
+      <c r="D116" s="15"/>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C117" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="13"/>
-    </row>
-    <row r="118" spans="2:4" ht="27" customHeight="1">
+      <c r="C117" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" s="15"/>
+    </row>
+    <row r="118" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D118" s="17"/>
     </row>
-    <row r="119" spans="2:4">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C119" s="5" t="s">
+      <c r="D119" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D119" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" ht="25.5">
+    </row>
+    <row r="120" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B120" s="6">
         <v>1</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4" ht="25.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B121" s="6">
         <v>2</v>
       </c>
       <c r="C121" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D121" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D121" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="122" spans="2:4" s="3" customFormat="1">
-      <c r="B122" s="14"/>
-      <c r="C122" s="15"/>
-      <c r="D122" s="15"/>
-    </row>
-    <row r="124" spans="2:4">
+    </row>
+    <row r="122" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="12"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" s="12">
+        <v>14</v>
+      </c>
+      <c r="C124" s="14">
         <v>16</v>
       </c>
-      <c r="D124" s="13"/>
-    </row>
-    <row r="125" spans="2:4">
+      <c r="D124" s="15"/>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C125" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D125" s="13"/>
-    </row>
-    <row r="126" spans="2:4" ht="25.5" customHeight="1">
+      <c r="C125" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="15"/>
+    </row>
+    <row r="126" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D126" s="17"/>
     </row>
-    <row r="127" spans="2:4">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="D127" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D127" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="128" spans="2:4" ht="25.5">
+    </row>
+    <row r="128" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B128" s="8">
         <v>1</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4" ht="25.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B129" s="8">
         <v>2</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="130" spans="2:4" s="3" customFormat="1">
-      <c r="B130" s="14"/>
-      <c r="C130" s="15"/>
-      <c r="D130" s="15"/>
-    </row>
-    <row r="132" spans="2:4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="12"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C132" s="12">
+        <v>14</v>
+      </c>
+      <c r="C132" s="14">
         <v>17</v>
       </c>
-      <c r="D132" s="13"/>
-    </row>
-    <row r="133" spans="2:4">
+      <c r="D132" s="15"/>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C133" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D133" s="13"/>
-    </row>
-    <row r="134" spans="2:4" ht="27" customHeight="1">
+      <c r="C133" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133" s="15"/>
+    </row>
+    <row r="134" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C134" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D134" s="17"/>
     </row>
-    <row r="135" spans="2:4">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C135" s="5" t="s">
+      <c r="D135" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D135" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="136" spans="2:4" ht="25.5">
+    </row>
+    <row r="136" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B136" s="8">
         <v>1</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="137" spans="2:4" ht="25.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B137" s="8">
         <v>2</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="138" spans="2:4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="8">
         <v>3</v>
       </c>
       <c r="C138" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D138" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D138" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="139" spans="2:4">
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="8">
         <v>4</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="140" spans="2:4" ht="25.5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B140" s="8">
         <v>5</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="141" spans="2:4" s="3" customFormat="1">
-      <c r="B141" s="14"/>
-      <c r="C141" s="15"/>
-      <c r="D141" s="15"/>
-    </row>
-    <row r="143" spans="2:4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="12"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C143" s="12">
+        <v>14</v>
+      </c>
+      <c r="C143" s="14">
         <v>18</v>
       </c>
-      <c r="D143" s="13"/>
-    </row>
-    <row r="144" spans="2:4">
+      <c r="D143" s="15"/>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C144" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D144" s="13"/>
-    </row>
-    <row r="145" spans="2:4" ht="27" customHeight="1">
+      <c r="C144" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D144" s="15"/>
+    </row>
+    <row r="145" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C145" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D145" s="17"/>
     </row>
-    <row r="146" spans="2:4">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C146" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="D146" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D146" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="147" spans="2:4" ht="25.5">
+    </row>
+    <row r="147" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B147" s="8">
         <v>1</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4" s="3" customFormat="1">
-      <c r="B148" s="14"/>
-      <c r="C148" s="15"/>
-      <c r="D148" s="15"/>
-    </row>
-    <row r="150" spans="2:4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="12"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C150" s="12">
+        <v>14</v>
+      </c>
+      <c r="C150" s="14">
         <v>19</v>
       </c>
-      <c r="D150" s="13"/>
-    </row>
-    <row r="151" spans="2:4">
+      <c r="D150" s="15"/>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C151" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D151" s="13"/>
-    </row>
-    <row r="152" spans="2:4" ht="28.5" customHeight="1">
+      <c r="C151" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151" s="15"/>
+    </row>
+    <row r="152" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D152" s="17"/>
     </row>
-    <row r="153" spans="2:4">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C153" s="5" t="s">
+      <c r="D153" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D153" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="154" spans="2:4" ht="25.5">
+    </row>
+    <row r="154" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B154" s="8">
         <v>1</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D154" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4" ht="25.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B155" s="8">
         <v>2</v>
       </c>
       <c r="C155" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D155" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D155" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="156" spans="2:4" s="3" customFormat="1">
-      <c r="B156" s="14"/>
-      <c r="C156" s="15"/>
-      <c r="D156" s="15"/>
-    </row>
-    <row r="158" spans="2:4">
+    </row>
+    <row r="156" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="12"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C158" s="12">
+        <v>14</v>
+      </c>
+      <c r="C158" s="14">
         <v>20</v>
       </c>
-      <c r="D158" s="13"/>
-    </row>
-    <row r="159" spans="2:4">
+      <c r="D158" s="15"/>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C159" s="12" t="s">
+      <c r="C159" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D159" s="15"/>
+    </row>
+    <row r="160" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C160" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D160" s="17"/>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D159" s="13"/>
-    </row>
-    <row r="160" spans="2:4" ht="29.25" customHeight="1">
-      <c r="B160" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C160" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D160" s="17"/>
-    </row>
-    <row r="161" spans="2:4">
-      <c r="B161" s="5" t="s">
+      <c r="C161" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C161" s="5" t="s">
+      <c r="D161" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D161" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" ht="25.5">
+    </row>
+    <row r="162" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B162" s="6">
         <v>1</v>
       </c>
       <c r="C162" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D162" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" ht="25.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B163" s="6">
         <v>2</v>
       </c>
       <c r="C163" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D163" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D163" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" s="3" customFormat="1">
-      <c r="B164" s="20"/>
-      <c r="C164" s="21"/>
-      <c r="D164" s="21"/>
+    </row>
+    <row r="164" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="18"/>
+      <c r="C164" s="19"/>
+      <c r="D164" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="B122:D122"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="B130:D130"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="B141:D141"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="B164:D164"/>
+    <mergeCell ref="C150:D150"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="B156:D156"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C159:D159"/>
     <mergeCell ref="B148:D148"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B23:D23"/>
@@ -2375,70 +2449,6 @@
     <mergeCell ref="C124:D124"/>
     <mergeCell ref="C125:D125"/>
     <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C160:D160"/>
-    <mergeCell ref="B164:D164"/>
-    <mergeCell ref="C150:D150"/>
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="B156:D156"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="C159:D159"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="B130:D130"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>